<commit_message>
update import file server
</commit_message>
<xml_diff>
--- a/report/QueBX_report.xlsx
+++ b/report/QueBX_report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="21930" windowHeight="12510" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView windowWidth="21930" windowHeight="12450" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="20200825" sheetId="1" r:id="rId1"/>
@@ -82,11 +82,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;\ _₫_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;\ &quot;₫&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₫_-;\-* #,##0.00\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;\ _₫_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -107,6 +107,154 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -116,154 +264,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -280,19 +280,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -304,6 +418,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -316,109 +442,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -431,30 +455,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -569,6 +569,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -598,21 +613,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -669,138 +669,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="15" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="15" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="14" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="12" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="14" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="13" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="13" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="12" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="13" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2091,7 +2091,7 @@
   <dimension ref="C5:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelCol="6"/>

</xml_diff>